<commit_message>
testadd new fileadd new file
</commit_message>
<xml_diff>
--- a/test/Test.xlsx
+++ b/test/Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Bed vovka</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>sdfsdf</t>
+  </si>
+  <si>
+    <t>wefwef</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -405,6 +408,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>